<commit_message>
📋: add grok patterns
</commit_message>
<xml_diff>
--- a/pattern.xlsx
+++ b/pattern.xlsx
@@ -42,7 +42,7 @@
     <t>%{IPV4:source.address} - - \[%{HTTPDATE:http.date}\] \"%{WORD:http.request.method} %{URIPATH:url.path}%{URIPARAM:url.param} HTTP\/%{BASE10NUM:http.version}\" %{INT:http.response.status_code} %{INT:http.response.bytes} \"-\" \"%{GREEDYDATA:user_agent.original}\"</t>
   </si>
   <si>
-    <t>Ngnix 3</t>
+    <t>Nginx 3</t>
   </si>
   <si>
     <t>%{IPV4:source.address} - - \[%{HTTPDATE:http.date}\] \"%{WORD:http.request.method} %{URIPATH:url.path}%{URIPARAM:url.param} HTTP\/%{BASE10NUM:http.version}\" %{INT:http.response.status_code} %{INT:http.response.bytes} \"%{URI:http.request.referrer}\" \"%{GREEDYDATA:user_agent.original}\"</t>
@@ -78,7 +78,7 @@
     <t>%{IPV4:source.address} - - \[%{HTTPDATE:http.date}\] %{INT} \"%{WORD:http.request.method} %{PATH:url.path} HTTP\/%{BASE10NUM:http.version}\" %{INT:http.response.status_code} %{INT:http.response.bytes} \"-\" \"%{GREEDYDATA:user_agent.original}\"</t>
   </si>
   <si>
-    <t xml:space="preserve">Apache 3 </t>
+    <t>Apache 3</t>
   </si>
   <si>
     <t>%{IPV4:source.address} - - \[%{HTTPDATE:http.date}\] %{INT} \"%{WORD:http.request.method} %{PATH:url.path} HTTP\/%{BASE10NUM:http.version}\" %{INT:http.response.status_code} %{INT:http.response.bytes}\"%{URI:http.request.referrer}\" \"%{GREEDYDATA:user_agent.original}\"</t>
@@ -132,11 +132,14 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
@@ -411,7 +414,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="8.71"/>
+    <col customWidth="1" min="1" max="1" width="25.86"/>
     <col customWidth="1" min="2" max="2" width="249.0"/>
     <col customWidth="1" min="3" max="3" width="240.43"/>
     <col customWidth="1" min="4" max="26" width="8.71"/>
@@ -450,7 +453,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -498,7 +501,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -517,7 +520,7 @@
       <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="3" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>